<commit_message>
Add choosing saving directory & fix some bugs (?)
</commit_message>
<xml_diff>
--- a/demo/calendar1.xlsx
+++ b/demo/calendar1.xlsx
@@ -271,24 +271,26 @@
     </font>
     <font>
       <name val="Comic Sans MS"/>
-      <color rgb="00FF0000"/>
-      <sz val="20"/>
+      <color rgb="00000000"/>
+      <sz val="24"/>
+    </font>
+    <font>
+      <color rgb="00000000"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Comic Sans MS"/>
-      <color rgb="00000000"/>
-      <sz val="20"/>
+      <color rgb="00FF0000"/>
+      <sz val="24"/>
     </font>
     <font>
       <name val="Comic Sans MS"/>
       <color rgb="000000FF"/>
-      <sz val="20"/>
+      <sz val="24"/>
     </font>
     <font>
       <color rgb="00FF0000"/>
-    </font>
-    <font>
-      <color rgb="00000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -354,25 +356,25 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -920,10 +922,10 @@
       <c r="C12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="9" t="n"/>
-      <c r="E12" s="9" t="n"/>
-      <c r="F12" s="9" t="n"/>
-      <c r="G12" s="9" t="n"/>
+      <c r="D12" s="11" t="n"/>
+      <c r="E12" s="11" t="n"/>
+      <c r="F12" s="11" t="n"/>
+      <c r="G12" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1184,10 +1186,10 @@
       <c r="C12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="9" t="n"/>
-      <c r="E12" s="9" t="n"/>
-      <c r="F12" s="9" t="n"/>
-      <c r="G12" s="9" t="n"/>
+      <c r="D12" s="11" t="n"/>
+      <c r="E12" s="11" t="n"/>
+      <c r="F12" s="11" t="n"/>
+      <c r="G12" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1257,9 +1259,9 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n"/>
-      <c r="B4" s="9" t="n"/>
-      <c r="C4" s="9" t="n"/>
+      <c r="A4" s="11" t="n"/>
+      <c r="B4" s="11" t="n"/>
+      <c r="C4" s="11" t="n"/>
       <c r="D4" s="9" t="s">
         <v>66</v>
       </c>
@@ -1446,8 +1448,8 @@
       <c r="E12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="9" t="n"/>
-      <c r="G12" s="9" t="n"/>
+      <c r="F12" s="11" t="n"/>
+      <c r="G12" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1513,11 +1515,11 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n"/>
-      <c r="B4" s="9" t="n"/>
-      <c r="C4" s="9" t="n"/>
-      <c r="D4" s="9" t="n"/>
-      <c r="E4" s="9" t="n"/>
+      <c r="A4" s="11" t="n"/>
+      <c r="B4" s="11" t="n"/>
+      <c r="C4" s="11" t="n"/>
+      <c r="D4" s="11" t="n"/>
+      <c r="E4" s="11" t="n"/>
       <c r="F4" s="9" t="s">
         <v>68</v>
       </c>
@@ -1724,12 +1726,12 @@
       <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="9" t="n"/>
-      <c r="C14" s="9" t="n"/>
-      <c r="D14" s="9" t="n"/>
-      <c r="E14" s="9" t="n"/>
-      <c r="F14" s="9" t="n"/>
-      <c r="G14" s="9" t="n"/>
+      <c r="B14" s="11" t="n"/>
+      <c r="C14" s="11" t="n"/>
+      <c r="D14" s="11" t="n"/>
+      <c r="E14" s="11" t="n"/>
+      <c r="F14" s="11" t="n"/>
+      <c r="G14" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1799,9 +1801,9 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n"/>
-      <c r="B4" s="9" t="n"/>
-      <c r="C4" s="9" t="n"/>
+      <c r="A4" s="11" t="n"/>
+      <c r="B4" s="11" t="n"/>
+      <c r="C4" s="11" t="n"/>
       <c r="D4" s="9" t="s">
         <v>41</v>
       </c>
@@ -1891,7 +1893,7 @@
       <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -1978,10 +1980,10 @@
       <c r="C12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="9" t="n"/>
-      <c r="E12" s="9" t="n"/>
-      <c r="F12" s="9" t="n"/>
-      <c r="G12" s="9" t="n"/>
+      <c r="D12" s="11" t="n"/>
+      <c r="E12" s="11" t="n"/>
+      <c r="F12" s="11" t="n"/>
+      <c r="G12" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2051,9 +2053,9 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n"/>
-      <c r="B4" s="9" t="n"/>
-      <c r="C4" s="9" t="n"/>
+      <c r="A4" s="11" t="n"/>
+      <c r="B4" s="11" t="n"/>
+      <c r="C4" s="11" t="n"/>
       <c r="D4" s="9" t="s">
         <v>44</v>
       </c>
@@ -2245,7 +2247,7 @@
       <c r="F12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="9" t="n"/>
+      <c r="G12" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2309,12 +2311,12 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n"/>
-      <c r="B4" s="9" t="n"/>
-      <c r="C4" s="9" t="n"/>
-      <c r="D4" s="9" t="n"/>
-      <c r="E4" s="9" t="n"/>
-      <c r="F4" s="9" t="n"/>
+      <c r="A4" s="11" t="n"/>
+      <c r="B4" s="11" t="n"/>
+      <c r="C4" s="11" t="n"/>
+      <c r="D4" s="11" t="n"/>
+      <c r="E4" s="11" t="n"/>
+      <c r="F4" s="11" t="n"/>
       <c r="G4" s="9" t="s">
         <v>47</v>
       </c>
@@ -2518,12 +2520,12 @@
       <c r="A14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="9" t="n"/>
-      <c r="C14" s="9" t="n"/>
-      <c r="D14" s="9" t="n"/>
-      <c r="E14" s="9" t="n"/>
-      <c r="F14" s="9" t="n"/>
-      <c r="G14" s="9" t="n"/>
+      <c r="B14" s="11" t="n"/>
+      <c r="C14" s="11" t="n"/>
+      <c r="D14" s="11" t="n"/>
+      <c r="E14" s="11" t="n"/>
+      <c r="F14" s="11" t="n"/>
+      <c r="G14" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2597,7 +2599,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n"/>
+      <c r="A4" s="11" t="n"/>
       <c r="B4" s="9" t="s">
         <v>50</v>
       </c>
@@ -2785,9 +2787,9 @@
       <c r="D12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="9" t="n"/>
-      <c r="F12" s="9" t="n"/>
-      <c r="G12" s="9" t="n"/>
+      <c r="E12" s="11" t="n"/>
+      <c r="F12" s="11" t="n"/>
+      <c r="G12" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2855,10 +2857,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n"/>
-      <c r="B4" s="9" t="n"/>
-      <c r="C4" s="9" t="n"/>
-      <c r="D4" s="9" t="n"/>
+      <c r="A4" s="11" t="n"/>
+      <c r="B4" s="11" t="n"/>
+      <c r="C4" s="11" t="n"/>
+      <c r="D4" s="11" t="n"/>
       <c r="E4" s="9" t="s">
         <v>53</v>
       </c>
@@ -3047,7 +3049,7 @@
       <c r="F12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="9" t="n"/>
+      <c r="G12" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -3111,12 +3113,12 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n"/>
-      <c r="B4" s="9" t="n"/>
-      <c r="C4" s="9" t="n"/>
-      <c r="D4" s="9" t="n"/>
-      <c r="E4" s="9" t="n"/>
-      <c r="F4" s="9" t="n"/>
+      <c r="A4" s="11" t="n"/>
+      <c r="B4" s="11" t="n"/>
+      <c r="C4" s="11" t="n"/>
+      <c r="D4" s="11" t="n"/>
+      <c r="E4" s="11" t="n"/>
+      <c r="F4" s="11" t="n"/>
       <c r="G4" s="9" t="s">
         <v>56</v>
       </c>
@@ -3325,11 +3327,11 @@
       <c r="B14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="9" t="n"/>
-      <c r="D14" s="9" t="n"/>
-      <c r="E14" s="9" t="n"/>
-      <c r="F14" s="9" t="n"/>
-      <c r="G14" s="9" t="n"/>
+      <c r="C14" s="11" t="n"/>
+      <c r="D14" s="11" t="n"/>
+      <c r="E14" s="11" t="n"/>
+      <c r="F14" s="11" t="n"/>
+      <c r="G14" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -3401,8 +3403,8 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n"/>
-      <c r="B4" s="9" t="n"/>
+      <c r="A4" s="11" t="n"/>
+      <c r="B4" s="11" t="n"/>
       <c r="C4" s="9" t="s">
         <v>59</v>
       </c>
@@ -3592,8 +3594,8 @@
       <c r="E12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="9" t="n"/>
-      <c r="G12" s="9" t="n"/>
+      <c r="F12" s="11" t="n"/>
+      <c r="G12" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -3659,11 +3661,11 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n"/>
-      <c r="B4" s="9" t="n"/>
-      <c r="C4" s="9" t="n"/>
-      <c r="D4" s="9" t="n"/>
-      <c r="E4" s="9" t="n"/>
+      <c r="A4" s="11" t="n"/>
+      <c r="B4" s="11" t="n"/>
+      <c r="C4" s="11" t="n"/>
+      <c r="D4" s="11" t="n"/>
+      <c r="E4" s="11" t="n"/>
       <c r="F4" s="9" t="s">
         <v>62</v>
       </c>
@@ -3865,13 +3867,13 @@
       <c r="G13" s="10" t="n"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="9" t="n"/>
-      <c r="B14" s="9" t="n"/>
-      <c r="C14" s="9" t="n"/>
-      <c r="D14" s="9" t="n"/>
-      <c r="E14" s="9" t="n"/>
-      <c r="F14" s="9" t="n"/>
-      <c r="G14" s="9" t="n"/>
+      <c r="A14" s="11" t="n"/>
+      <c r="B14" s="11" t="n"/>
+      <c r="C14" s="11" t="n"/>
+      <c r="D14" s="11" t="n"/>
+      <c r="E14" s="11" t="n"/>
+      <c r="F14" s="11" t="n"/>
+      <c r="G14" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>